<commit_message>
Server: xlnt 오류 수정
</commit_message>
<xml_diff>
--- a/Client/Assets/11. GameData/Mode_Ver3.xlsx
+++ b/Client/Assets/11. GameData/Mode_Ver3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1DA6AD-10DA-4283-A3EA-594244612711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4E3641-6216-4E4A-9461-E2938C0F6A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="490" activeTab="2" xr2:uid="{00881117-46AD-47BC-AC4E-DE2587EC70E9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="490" activeTab="2" xr2:uid="{00881117-46AD-47BC-AC4E-DE2587EC70E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Matching" sheetId="10" r:id="rId1"/>
@@ -494,7 +494,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="77">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -801,10 +801,6 @@
   </si>
   <si>
     <t>FITH_Team_Battle_6_Draw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1517,22 +1513,22 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.58203125" customWidth="1"/>
-    <col min="7" max="7" width="13.9140625" customWidth="1"/>
-    <col min="8" max="9" width="24.4140625" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="7" width="13.875" customWidth="1"/>
+    <col min="8" max="9" width="24.375" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>66</v>
       </c>
@@ -1552,7 +1548,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>110</v>
       </c>
@@ -1572,7 +1568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>110</v>
       </c>
@@ -1592,7 +1588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>110</v>
       </c>
@@ -1612,7 +1608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>120</v>
       </c>
@@ -1632,7 +1628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>120</v>
       </c>
@@ -1652,7 +1648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>120</v>
       </c>
@@ -1685,22 +1681,22 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>111</v>
       </c>
@@ -1758,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>112</v>
       </c>
@@ -1787,7 +1783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>121</v>
       </c>
@@ -1816,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>122</v>
       </c>
@@ -1857,42 +1853,42 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.08203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.08203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.08203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.08203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.08203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.75" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1963,7 +1959,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>111</v>
       </c>
@@ -2034,7 +2030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>112</v>
       </c>
@@ -2096,7 +2092,7 @@
         <v>3002</v>
       </c>
       <c r="U3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="V3">
         <v>10</v>
@@ -2105,7 +2101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>121</v>
       </c>
@@ -2167,7 +2163,7 @@
         <v>3002</v>
       </c>
       <c r="U4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="V4">
         <v>10</v>
@@ -2176,7 +2172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>122</v>
       </c>
@@ -2238,7 +2234,7 @@
         <v>3002</v>
       </c>
       <c r="U5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="V5">
         <v>10</v>
@@ -2247,15 +2243,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
         <v>46</v>
       </c>
@@ -2271,22 +2264,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AB955C-74DD-4B61-BCC6-9955AD17436D}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:G37"/>
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.58203125" customWidth="1"/>
+    <col min="7" max="7" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2302,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>111101</v>
       </c>
@@ -2332,7 +2325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>111102</v>
       </c>
@@ -2355,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>111103</v>
       </c>
@@ -2378,7 +2371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>111201</v>
       </c>
@@ -2401,7 +2394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>111202</v>
       </c>
@@ -2424,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>111203</v>
       </c>
@@ -2447,7 +2440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>111301</v>
       </c>
@@ -2470,7 +2463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>111302</v>
       </c>
@@ -2493,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>111303</v>
       </c>
@@ -2516,7 +2509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>112101</v>
       </c>
@@ -2539,7 +2532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>112102</v>
       </c>
@@ -2562,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>112103</v>
       </c>
@@ -2585,7 +2578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>112201</v>
       </c>
@@ -2608,7 +2601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>112202</v>
       </c>
@@ -2631,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>112203</v>
       </c>
@@ -2654,7 +2647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>112301</v>
       </c>
@@ -2677,7 +2670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>112302</v>
       </c>
@@ -2700,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>112303</v>
       </c>
@@ -2723,7 +2716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>113101</v>
       </c>
@@ -2746,7 +2739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>113102</v>
       </c>
@@ -2769,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>113103</v>
       </c>
@@ -2792,7 +2785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>113201</v>
       </c>
@@ -2815,7 +2808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>113202</v>
       </c>
@@ -2838,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>113203</v>
       </c>
@@ -2861,7 +2854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>113301</v>
       </c>
@@ -2884,7 +2877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>113302</v>
       </c>
@@ -2907,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>113303</v>
       </c>
@@ -2930,7 +2923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>121101</v>
       </c>
@@ -2953,7 +2946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>121102</v>
       </c>
@@ -2976,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>121103</v>
       </c>
@@ -2999,7 +2992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>121201</v>
       </c>
@@ -3022,7 +3015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>121202</v>
       </c>
@@ -3045,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>121203</v>
       </c>
@@ -3068,7 +3061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>121301</v>
       </c>
@@ -3091,7 +3084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>121302</v>
       </c>
@@ -3114,7 +3107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>121303</v>
       </c>
@@ -3137,7 +3130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>122101</v>
       </c>
@@ -3160,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>122102</v>
       </c>
@@ -3183,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>122103</v>
       </c>
@@ -3206,7 +3199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>122201</v>
       </c>
@@ -3229,7 +3222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>122202</v>
       </c>
@@ -3252,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>122203</v>
       </c>
@@ -3275,7 +3268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>122301</v>
       </c>
@@ -3298,7 +3291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>122302</v>
       </c>
@@ -3321,7 +3314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>122303</v>
       </c>
@@ -3344,39 +3337,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
     </row>
@@ -3392,19 +3385,19 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3436,7 +3429,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>111001</v>
       </c>
@@ -3468,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>111002</v>
       </c>
@@ -3500,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>111003</v>
       </c>
@@ -3532,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>112001</v>
       </c>
@@ -3564,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>112002</v>
       </c>
@@ -3596,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>112003</v>
       </c>
@@ -3628,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>113001</v>
       </c>
@@ -3660,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>113002</v>
       </c>
@@ -3692,7 +3685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>113003</v>
       </c>
@@ -3724,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>121001</v>
       </c>
@@ -3756,7 +3749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>121002</v>
       </c>
@@ -3788,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>121003</v>
       </c>
@@ -3820,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>122001</v>
       </c>
@@ -3852,7 +3845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>121002</v>
       </c>
@@ -3884,7 +3877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>121003</v>
       </c>
@@ -3916,47 +3909,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
     </row>
@@ -3972,21 +3965,21 @@
   <dimension ref="A1:L171"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M152" sqref="M152"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N166" sqref="N166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4024,7 +4017,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>111100</v>
       </c>
@@ -4062,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>111101</v>
       </c>
@@ -4100,7 +4093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>111102</v>
       </c>
@@ -4138,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>111103</v>
       </c>
@@ -4176,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>111104</v>
       </c>
@@ -4214,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>111105</v>
       </c>
@@ -4252,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>111106</v>
       </c>
@@ -4290,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>111107</v>
       </c>
@@ -4328,7 +4321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>111108</v>
       </c>
@@ -4366,7 +4359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>111109</v>
       </c>
@@ -4404,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>111110</v>
       </c>
@@ -4442,7 +4435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>111111</v>
       </c>
@@ -4480,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>111200</v>
       </c>
@@ -4518,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>111201</v>
       </c>
@@ -4556,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>111202</v>
       </c>
@@ -4594,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>111203</v>
       </c>
@@ -4632,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>111204</v>
       </c>
@@ -4670,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>111205</v>
       </c>
@@ -4708,7 +4701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>111206</v>
       </c>
@@ -4746,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>111207</v>
       </c>
@@ -4784,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>111208</v>
       </c>
@@ -4822,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>111209</v>
       </c>
@@ -4860,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>111210</v>
       </c>
@@ -4898,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>111300</v>
       </c>
@@ -4936,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>111301</v>
       </c>
@@ -4974,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>111302</v>
       </c>
@@ -5012,7 +5005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>111303</v>
       </c>
@@ -5050,7 +5043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>111304</v>
       </c>
@@ -5088,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>111305</v>
       </c>
@@ -5126,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>111306</v>
       </c>
@@ -5164,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>111307</v>
       </c>
@@ -5202,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>111308</v>
       </c>
@@ -5240,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>111309</v>
       </c>
@@ -5278,7 +5271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>111310</v>
       </c>
@@ -5316,7 +5309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>112100</v>
       </c>
@@ -5354,7 +5347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>112101</v>
       </c>
@@ -5392,7 +5385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>112102</v>
       </c>
@@ -5430,7 +5423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>112103</v>
       </c>
@@ -5468,7 +5461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>112104</v>
       </c>
@@ -5506,7 +5499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>112105</v>
       </c>
@@ -5544,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>112106</v>
       </c>
@@ -5582,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>112107</v>
       </c>
@@ -5620,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>112108</v>
       </c>
@@ -5658,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>112109</v>
       </c>
@@ -5696,7 +5689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>112110</v>
       </c>
@@ -5734,7 +5727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>112111</v>
       </c>
@@ -5772,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>112200</v>
       </c>
@@ -5810,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>112201</v>
       </c>
@@ -5848,7 +5841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>112202</v>
       </c>
@@ -5886,7 +5879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>112203</v>
       </c>
@@ -5924,7 +5917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>112204</v>
       </c>
@@ -5962,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>112205</v>
       </c>
@@ -6000,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>112206</v>
       </c>
@@ -6038,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>112207</v>
       </c>
@@ -6076,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>112208</v>
       </c>
@@ -6114,7 +6107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>112209</v>
       </c>
@@ -6152,7 +6145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>112210</v>
       </c>
@@ -6190,7 +6183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>112300</v>
       </c>
@@ -6228,7 +6221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>112301</v>
       </c>
@@ -6266,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>112302</v>
       </c>
@@ -6304,7 +6297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>112303</v>
       </c>
@@ -6342,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>112304</v>
       </c>
@@ -6380,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>112305</v>
       </c>
@@ -6418,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>112306</v>
       </c>
@@ -6456,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>112307</v>
       </c>
@@ -6494,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>112308</v>
       </c>
@@ -6532,7 +6525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>112309</v>
       </c>
@@ -6570,7 +6563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>112310</v>
       </c>
@@ -6608,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>113100</v>
       </c>
@@ -6646,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>113101</v>
       </c>
@@ -6684,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>113102</v>
       </c>
@@ -6722,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>113103</v>
       </c>
@@ -6760,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>113104</v>
       </c>
@@ -6798,7 +6791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>113105</v>
       </c>
@@ -6836,7 +6829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>113106</v>
       </c>
@@ -6874,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>113107</v>
       </c>
@@ -6912,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>113108</v>
       </c>
@@ -6950,7 +6943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>113109</v>
       </c>
@@ -6988,7 +6981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>113110</v>
       </c>
@@ -7026,7 +7019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>113111</v>
       </c>
@@ -7064,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>113200</v>
       </c>
@@ -7102,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>113201</v>
       </c>
@@ -7140,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>113202</v>
       </c>
@@ -7178,7 +7171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>113203</v>
       </c>
@@ -7216,7 +7209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>113204</v>
       </c>
@@ -7254,7 +7247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>113205</v>
       </c>
@@ -7292,7 +7285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>113206</v>
       </c>
@@ -7330,7 +7323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>113207</v>
       </c>
@@ -7368,7 +7361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>113208</v>
       </c>
@@ -7406,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>113209</v>
       </c>
@@ -7444,7 +7437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>113210</v>
       </c>
@@ -7482,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>113300</v>
       </c>
@@ -7520,7 +7513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>113301</v>
       </c>
@@ -7558,7 +7551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <v>113302</v>
       </c>
@@ -7596,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>113303</v>
       </c>
@@ -7634,7 +7627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>113304</v>
       </c>
@@ -7672,7 +7665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>113305</v>
       </c>
@@ -7710,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>113306</v>
       </c>
@@ -7748,7 +7741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>113307</v>
       </c>
@@ -7786,7 +7779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="6">
         <v>113308</v>
       </c>
@@ -7824,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="6">
         <v>113309</v>
       </c>
@@ -7862,7 +7855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="6">
         <v>113310</v>
       </c>
@@ -7900,7 +7893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="6">
         <v>121100</v>
       </c>
@@ -7938,7 +7931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>121101</v>
       </c>
@@ -7976,7 +7969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>121102</v>
       </c>
@@ -8014,7 +8007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>121103</v>
       </c>
@@ -8052,7 +8045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="6">
         <v>121104</v>
       </c>
@@ -8090,7 +8083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="6">
         <v>121105</v>
       </c>
@@ -8128,7 +8121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="6">
         <v>121106</v>
       </c>
@@ -8166,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="6">
         <v>121107</v>
       </c>
@@ -8204,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
         <v>121108</v>
       </c>
@@ -8242,7 +8235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
         <v>121109</v>
       </c>
@@ -8280,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="6">
         <v>121110</v>
       </c>
@@ -8318,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="6">
         <v>121111</v>
       </c>
@@ -8356,7 +8349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>121200</v>
       </c>
@@ -8394,7 +8387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="6">
         <v>121201</v>
       </c>
@@ -8432,7 +8425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="6">
         <v>121202</v>
       </c>
@@ -8470,7 +8463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="6">
         <v>121203</v>
       </c>
@@ -8508,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
         <v>121204</v>
       </c>
@@ -8546,7 +8539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="6">
         <v>121205</v>
       </c>
@@ -8584,7 +8577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="6">
         <v>121206</v>
       </c>
@@ -8622,7 +8615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="6">
         <v>121207</v>
       </c>
@@ -8660,7 +8653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="6">
         <v>121208</v>
       </c>
@@ -8698,7 +8691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="6">
         <v>121209</v>
       </c>
@@ -8736,7 +8729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="6">
         <v>121210</v>
       </c>
@@ -8774,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="6">
         <v>121300</v>
       </c>
@@ -8812,7 +8805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="6">
         <v>121301</v>
       </c>
@@ -8850,7 +8843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="6">
         <v>121302</v>
       </c>
@@ -8888,7 +8881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="6">
         <v>121303</v>
       </c>
@@ -8926,7 +8919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="6">
         <v>121304</v>
       </c>
@@ -8964,7 +8957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="6">
         <v>121305</v>
       </c>
@@ -9002,7 +8995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="6">
         <v>121306</v>
       </c>
@@ -9040,7 +9033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="6">
         <v>121307</v>
       </c>
@@ -9078,7 +9071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="6">
         <v>121308</v>
       </c>
@@ -9116,7 +9109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="6">
         <v>121309</v>
       </c>
@@ -9154,7 +9147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="6">
         <v>121310</v>
       </c>
@@ -9192,7 +9185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="6">
         <v>122100</v>
       </c>
@@ -9230,7 +9223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="6">
         <v>122101</v>
       </c>
@@ -9268,7 +9261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="6">
         <v>122102</v>
       </c>
@@ -9306,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="6">
         <v>122103</v>
       </c>
@@ -9344,7 +9337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="6">
         <v>122104</v>
       </c>
@@ -9382,7 +9375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="6">
         <v>122105</v>
       </c>
@@ -9420,7 +9413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="6">
         <v>122106</v>
       </c>
@@ -9458,7 +9451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="6">
         <v>122107</v>
       </c>
@@ -9496,7 +9489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="6">
         <v>122108</v>
       </c>
@@ -9534,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="6">
         <v>122109</v>
       </c>
@@ -9572,7 +9565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="6">
         <v>122110</v>
       </c>
@@ -9610,7 +9603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="6">
         <v>122111</v>
       </c>
@@ -9648,7 +9641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="6">
         <v>122200</v>
       </c>
@@ -9686,7 +9679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="6">
         <v>122201</v>
       </c>
@@ -9724,7 +9717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="6">
         <v>122202</v>
       </c>
@@ -9762,7 +9755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="6">
         <v>122203</v>
       </c>
@@ -9800,7 +9793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="6">
         <v>122204</v>
       </c>
@@ -9838,7 +9831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="6">
         <v>122205</v>
       </c>
@@ -9876,7 +9869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="6">
         <v>122206</v>
       </c>
@@ -9914,7 +9907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="6">
         <v>122207</v>
       </c>
@@ -9952,7 +9945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="6">
         <v>122208</v>
       </c>
@@ -9990,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="6">
         <v>122209</v>
       </c>
@@ -10028,7 +10021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="6">
         <v>122210</v>
       </c>
@@ -10066,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="6">
         <v>122300</v>
       </c>
@@ -10104,7 +10097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="6">
         <v>122301</v>
       </c>
@@ -10142,7 +10135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="6">
         <v>122302</v>
       </c>
@@ -10180,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="6">
         <v>122303</v>
       </c>
@@ -10218,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="6">
         <v>122304</v>
       </c>
@@ -10256,7 +10249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="6">
         <v>122305</v>
       </c>
@@ -10294,7 +10287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
         <v>122306</v>
       </c>
@@ -10332,7 +10325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="6">
         <v>122307</v>
       </c>
@@ -10370,7 +10363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="6">
         <v>122308</v>
       </c>
@@ -10408,7 +10401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
         <v>122309</v>
       </c>
@@ -10446,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="6">
         <v>122310</v>
       </c>

</xml_diff>

<commit_message>
Map_Index -> Index로 수정
</commit_message>
<xml_diff>
--- a/Client/Assets/11. GameData/Mode_Ver3.xlsx
+++ b/Client/Assets/11. GameData/Mode_Ver3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D730145-55D7-43AE-8610-4044A557A548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7470E4A0-4891-4037-BFF8-E1AD4A214ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="490" activeTab="2" xr2:uid="{00881117-46AD-47BC-AC4E-DE2587EC70E9}"/>
   </bookViews>
@@ -516,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="81">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -839,10 +839,6 @@
   </si>
   <si>
     <t>Bomb_Ready_Time2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1904,9 +1900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D1EFC-2C97-4775-89FB-1DF8061BC0EF}">
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB11" sqref="AB11"/>
+      <selection pane="topRight" activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1949,7 +1945,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>35</v>
@@ -2796,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AB955C-74DD-4B61-BCC6-9955AD17436D}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>